<commit_message>
created new version of prioritization report to move to final draft
</commit_message>
<xml_diff>
--- a/data/prioritization/iptds_site_recommendations_20240904.xlsx
+++ b/data/prioritization/iptds_site_recommendations_20240904.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\prioritization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5C0ECD-C710-4013-B67E-16DEAC132DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27A2CE5-E3D8-4722-B801-B06E062832B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$51</definedName>
     <definedName name="lat_lon">Sheet2!$A$1:$C$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -823,7 +824,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A25" sqref="A25:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1760,6 +1761,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F51" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>